<commit_message>
Add metro area geojson + data
</commit_message>
<xml_diff>
--- a/census-data/QC Completed 2011.xlsx
+++ b/census-data/QC Completed 2011.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilyankou/Desktop/etobicoke/census-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilyankou/etobicoke/census-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5C7049-C72F-5F44-B25C-0EBF8F5E0FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03732E7F-D4A8-AC41-85A7-673F751F2085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="11860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map and data source" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
   <si>
     <t>CT NAME</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Income and Occupation (I)</t>
+  </si>
+  <si>
+    <t>is_metro</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
         <v>23</v>
       </c>
@@ -763,257 +766,275 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="15" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="15" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="15"/>
+    <col min="1" max="2" width="18.5" style="15" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="380" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="380" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>200</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="20">
         <v>6360</v>
       </c>
-      <c r="C2" s="20">
+      <c r="D2" s="20">
         <v>3565</v>
       </c>
-      <c r="D2" s="20">
+      <c r="E2" s="20">
         <v>80</v>
       </c>
-      <c r="E2" s="20">
+      <c r="F2" s="20">
         <v>2095</v>
       </c>
-      <c r="F2" s="20">
-        <v>0</v>
-      </c>
       <c r="G2" s="20">
+        <v>0</v>
+      </c>
+      <c r="H2" s="20">
         <v>1390</v>
       </c>
-      <c r="H2" s="15">
+      <c r="I2" s="15">
         <v>5</v>
       </c>
-      <c r="I2" s="20">
+      <c r="J2" s="20">
         <v>80</v>
       </c>
-      <c r="J2" s="15">
+      <c r="K2" s="15">
         <v>15</v>
       </c>
-      <c r="K2" s="20">
+      <c r="L2" s="20">
         <v>1285</v>
       </c>
-      <c r="L2" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>201</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20">
         <v>4922</v>
       </c>
-      <c r="C3" s="20">
+      <c r="D3" s="20">
         <v>2590</v>
       </c>
-      <c r="D3" s="20">
+      <c r="E3" s="20">
         <v>340</v>
       </c>
-      <c r="E3" s="20">
+      <c r="F3" s="20">
         <v>1065</v>
       </c>
-      <c r="F3" s="20">
-        <v>0</v>
-      </c>
       <c r="G3" s="20">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20">
         <v>1175</v>
       </c>
-      <c r="H3" s="15">
+      <c r="I3" s="15">
         <v>75</v>
       </c>
-      <c r="I3" s="20">
+      <c r="J3" s="20">
         <v>335</v>
       </c>
-      <c r="J3" s="15">
+      <c r="K3" s="15">
         <v>80</v>
       </c>
-      <c r="K3" s="20">
+      <c r="L3" s="20">
         <v>685</v>
       </c>
-      <c r="L3" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>202</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20">
         <v>1640</v>
       </c>
-      <c r="C4" s="20">
+      <c r="D4" s="20">
         <v>635</v>
       </c>
-      <c r="D4" s="20">
+      <c r="E4" s="20">
         <v>435</v>
       </c>
-      <c r="E4" s="20">
-        <v>0</v>
-      </c>
       <c r="F4" s="20">
         <v>0</v>
       </c>
       <c r="G4" s="20">
+        <v>0</v>
+      </c>
+      <c r="H4" s="20">
         <v>200</v>
       </c>
-      <c r="H4" s="15">
+      <c r="I4" s="15">
         <v>10</v>
       </c>
-      <c r="I4" s="20">
-        <v>0</v>
-      </c>
-      <c r="J4" s="15">
+      <c r="J4" s="20">
+        <v>0</v>
+      </c>
+      <c r="K4" s="15">
         <v>55</v>
       </c>
-      <c r="K4" s="20">
+      <c r="L4" s="20">
         <v>135</v>
       </c>
-      <c r="L4" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>203</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20">
         <v>3017</v>
       </c>
-      <c r="C5" s="20">
+      <c r="D5" s="20">
         <v>1405</v>
       </c>
-      <c r="D5" s="20">
+      <c r="E5" s="20">
         <v>655</v>
       </c>
-      <c r="E5" s="20">
+      <c r="F5" s="20">
         <v>230</v>
       </c>
-      <c r="F5" s="20">
-        <v>0</v>
-      </c>
       <c r="G5" s="20">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
         <v>515</v>
       </c>
-      <c r="H5" s="15">
+      <c r="I5" s="15">
         <v>55</v>
       </c>
-      <c r="I5" s="20">
+      <c r="J5" s="20">
         <v>25</v>
       </c>
-      <c r="J5" s="15">
+      <c r="K5" s="15">
         <v>80</v>
       </c>
-      <c r="K5" s="20">
+      <c r="L5" s="20">
         <v>365</v>
       </c>
-      <c r="L5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>204</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="20">
         <v>4380</v>
       </c>
-      <c r="C6" s="20">
+      <c r="D6" s="20">
         <v>2180</v>
       </c>
-      <c r="D6" s="20">
+      <c r="E6" s="20">
         <v>905</v>
       </c>
-      <c r="E6" s="20">
+      <c r="F6" s="20">
         <v>365</v>
       </c>
-      <c r="F6" s="20">
-        <v>0</v>
-      </c>
       <c r="G6" s="20">
+        <v>0</v>
+      </c>
+      <c r="H6" s="20">
         <v>910</v>
       </c>
-      <c r="H6" s="15">
+      <c r="I6" s="15">
         <v>120</v>
       </c>
-      <c r="I6" s="20">
-        <v>0</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="J6" s="20">
+        <v>0</v>
+      </c>
+      <c r="K6" s="15">
         <v>95</v>
       </c>
-      <c r="K6" s="20">
+      <c r="L6" s="20">
         <v>695</v>
       </c>
-      <c r="L6" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>205</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="20">
         <v>184</v>
       </c>
-      <c r="C7" s="20">
-        <v>0</v>
-      </c>
       <c r="D7" s="20">
         <v>0</v>
       </c>
@@ -1026,2627 +1047,2846 @@
       <c r="G7" s="20">
         <v>0</v>
       </c>
-      <c r="H7" s="15">
-        <v>0</v>
-      </c>
-      <c r="I7" s="20">
-        <v>0</v>
-      </c>
-      <c r="J7" s="15">
-        <v>0</v>
-      </c>
-      <c r="K7" s="20">
-        <v>0</v>
-      </c>
-      <c r="L7" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="H7" s="20">
+        <v>0</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0</v>
+      </c>
+      <c r="J7" s="20">
+        <v>0</v>
+      </c>
+      <c r="K7" s="15">
+        <v>0</v>
+      </c>
+      <c r="L7" s="20">
+        <v>0</v>
+      </c>
+      <c r="M7" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>206.01</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="20">
         <v>3972</v>
       </c>
-      <c r="C8" s="20">
+      <c r="D8" s="20">
         <v>1900</v>
       </c>
-      <c r="D8" s="20">
+      <c r="E8" s="20">
         <v>595</v>
       </c>
-      <c r="E8" s="20">
+      <c r="F8" s="20">
         <v>320</v>
       </c>
-      <c r="F8" s="20">
-        <v>0</v>
-      </c>
       <c r="G8" s="20">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20">
         <v>985</v>
       </c>
-      <c r="H8" s="15">
+      <c r="I8" s="15">
         <v>40</v>
       </c>
-      <c r="I8" s="20">
-        <v>0</v>
-      </c>
-      <c r="J8" s="15">
+      <c r="J8" s="20">
+        <v>0</v>
+      </c>
+      <c r="K8" s="15">
         <v>80</v>
       </c>
-      <c r="K8" s="20">
+      <c r="L8" s="20">
         <v>860</v>
       </c>
-      <c r="L8" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M8" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>206.02</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="20">
         <v>5660</v>
       </c>
-      <c r="C9" s="20">
+      <c r="D9" s="20">
         <v>2615</v>
       </c>
-      <c r="D9" s="20">
+      <c r="E9" s="20">
         <v>920</v>
       </c>
-      <c r="E9" s="20">
+      <c r="F9" s="20">
         <v>600</v>
       </c>
-      <c r="F9" s="20">
-        <v>0</v>
-      </c>
       <c r="G9" s="20">
+        <v>0</v>
+      </c>
+      <c r="H9" s="20">
         <v>1095</v>
       </c>
-      <c r="H9" s="15">
+      <c r="I9" s="15">
         <v>45</v>
       </c>
-      <c r="I9" s="20">
+      <c r="J9" s="20">
         <v>90</v>
       </c>
-      <c r="J9" s="15">
+      <c r="K9" s="15">
         <v>120</v>
       </c>
-      <c r="K9" s="20">
+      <c r="L9" s="20">
         <v>835</v>
       </c>
-      <c r="L9" s="15">
+      <c r="M9" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>207</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="20">
         <v>2302</v>
       </c>
-      <c r="C10" s="20">
+      <c r="D10" s="20">
         <v>1025</v>
       </c>
-      <c r="D10" s="20">
+      <c r="E10" s="20">
         <v>500</v>
       </c>
-      <c r="E10" s="20">
+      <c r="F10" s="20">
         <v>5</v>
       </c>
-      <c r="F10" s="20">
-        <v>0</v>
-      </c>
       <c r="G10" s="20">
+        <v>0</v>
+      </c>
+      <c r="H10" s="20">
         <v>530</v>
       </c>
-      <c r="H10" s="15">
+      <c r="I10" s="15">
         <v>15</v>
       </c>
-      <c r="I10" s="20">
-        <v>0</v>
-      </c>
-      <c r="J10" s="15">
+      <c r="J10" s="20">
+        <v>0</v>
+      </c>
+      <c r="K10" s="15">
         <v>35</v>
       </c>
-      <c r="K10" s="20">
+      <c r="L10" s="20">
         <v>475</v>
       </c>
-      <c r="L10" s="15">
+      <c r="M10" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>208</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="20">
         <v>4034</v>
       </c>
-      <c r="C11" s="20">
+      <c r="D11" s="20">
         <v>1955</v>
       </c>
-      <c r="D11" s="20">
+      <c r="E11" s="20">
         <v>175</v>
       </c>
-      <c r="E11" s="20">
+      <c r="F11" s="20">
         <v>765</v>
       </c>
-      <c r="F11" s="20">
-        <v>0</v>
-      </c>
       <c r="G11" s="20">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20">
         <v>1020</v>
       </c>
-      <c r="H11" s="15">
+      <c r="I11" s="15">
         <v>65</v>
       </c>
-      <c r="I11" s="20">
+      <c r="J11" s="20">
         <v>240</v>
       </c>
-      <c r="J11" s="15">
+      <c r="K11" s="15">
         <v>55</v>
       </c>
-      <c r="K11" s="20">
+      <c r="L11" s="20">
         <v>650</v>
       </c>
-      <c r="L11" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M11" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>209</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="20">
         <v>2747</v>
       </c>
-      <c r="C12" s="20">
+      <c r="D12" s="20">
         <v>1305</v>
       </c>
-      <c r="D12" s="20">
+      <c r="E12" s="20">
         <v>385</v>
       </c>
-      <c r="E12" s="20">
+      <c r="F12" s="20">
         <v>300</v>
       </c>
-      <c r="F12" s="20">
-        <v>0</v>
-      </c>
       <c r="G12" s="20">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20">
         <v>625</v>
       </c>
-      <c r="H12" s="15">
+      <c r="I12" s="15">
         <v>65</v>
       </c>
-      <c r="I12" s="20">
+      <c r="J12" s="20">
         <v>35</v>
       </c>
-      <c r="J12" s="15">
+      <c r="K12" s="15">
         <v>90</v>
       </c>
-      <c r="K12" s="20">
+      <c r="L12" s="20">
         <v>435</v>
       </c>
-      <c r="L12" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M12" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>210</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="20">
         <v>7855</v>
       </c>
-      <c r="C13" s="20">
+      <c r="D13" s="20">
         <v>4185</v>
       </c>
-      <c r="D13" s="20">
+      <c r="E13" s="20">
         <v>405</v>
       </c>
-      <c r="E13" s="20">
+      <c r="F13" s="20">
         <v>3145</v>
       </c>
-      <c r="F13" s="20">
+      <c r="G13" s="20">
         <v>5</v>
       </c>
-      <c r="G13" s="20">
+      <c r="H13" s="20">
         <v>635</v>
       </c>
-      <c r="H13" s="15">
+      <c r="I13" s="15">
         <v>75</v>
       </c>
-      <c r="I13" s="20">
+      <c r="J13" s="20">
         <v>445</v>
       </c>
-      <c r="J13" s="15">
+      <c r="K13" s="15">
         <v>50</v>
       </c>
-      <c r="K13" s="20">
+      <c r="L13" s="20">
         <v>70</v>
       </c>
-      <c r="L13" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M13" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>211</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="20">
         <v>6286</v>
       </c>
-      <c r="C14" s="20">
+      <c r="D14" s="20">
         <v>2485</v>
       </c>
-      <c r="D14" s="20">
+      <c r="E14" s="20">
         <v>1455</v>
       </c>
-      <c r="E14" s="20">
+      <c r="F14" s="20">
         <v>240</v>
       </c>
-      <c r="F14" s="20">
-        <v>0</v>
-      </c>
       <c r="G14" s="20">
+        <v>0</v>
+      </c>
+      <c r="H14" s="20">
         <v>790</v>
       </c>
-      <c r="H14" s="15">
+      <c r="I14" s="15">
         <v>350</v>
       </c>
-      <c r="I14" s="20">
+      <c r="J14" s="20">
         <v>5</v>
       </c>
-      <c r="J14" s="15">
+      <c r="K14" s="15">
         <v>195</v>
       </c>
-      <c r="K14" s="20">
+      <c r="L14" s="20">
         <v>235</v>
       </c>
-      <c r="L14" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>212</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="20">
         <v>5618</v>
       </c>
-      <c r="C15" s="20">
+      <c r="D15" s="20">
         <v>2175</v>
       </c>
-      <c r="D15" s="20">
+      <c r="E15" s="20">
         <v>1395</v>
       </c>
-      <c r="E15" s="20">
+      <c r="F15" s="20">
         <v>85</v>
       </c>
-      <c r="F15" s="20">
-        <v>0</v>
-      </c>
       <c r="G15" s="20">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
         <v>690</v>
       </c>
-      <c r="H15" s="15">
+      <c r="I15" s="15">
         <v>170</v>
       </c>
-      <c r="I15" s="20">
+      <c r="J15" s="20">
         <v>80</v>
       </c>
-      <c r="J15" s="15">
+      <c r="K15" s="15">
         <v>130</v>
       </c>
-      <c r="K15" s="20">
+      <c r="L15" s="20">
         <v>305</v>
       </c>
-      <c r="L15" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>213</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20">
         <v>6792</v>
       </c>
-      <c r="C16" s="20">
+      <c r="D16" s="20">
         <v>3170</v>
       </c>
-      <c r="D16" s="20">
+      <c r="E16" s="20">
         <v>1015</v>
       </c>
-      <c r="E16" s="20">
+      <c r="F16" s="20">
         <v>2075</v>
       </c>
-      <c r="F16" s="20">
-        <v>0</v>
-      </c>
       <c r="G16" s="20">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20">
         <v>80</v>
       </c>
-      <c r="H16" s="15">
-        <v>0</v>
-      </c>
-      <c r="I16" s="20">
+      <c r="I16" s="15">
+        <v>0</v>
+      </c>
+      <c r="J16" s="20">
         <v>5</v>
       </c>
-      <c r="J16" s="15">
+      <c r="K16" s="15">
         <v>40</v>
       </c>
-      <c r="K16" s="20">
+      <c r="L16" s="20">
         <v>35</v>
       </c>
-      <c r="L16" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>214</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="20">
         <v>4307</v>
       </c>
-      <c r="C17" s="20">
+      <c r="D17" s="20">
         <v>1960</v>
       </c>
-      <c r="D17" s="20">
+      <c r="E17" s="20">
         <v>785</v>
       </c>
-      <c r="E17" s="20">
+      <c r="F17" s="20">
         <v>625</v>
       </c>
-      <c r="F17" s="20">
-        <v>0</v>
-      </c>
       <c r="G17" s="20">
+        <v>0</v>
+      </c>
+      <c r="H17" s="20">
         <v>550</v>
       </c>
-      <c r="H17" s="15">
+      <c r="I17" s="15">
         <v>65</v>
       </c>
-      <c r="I17" s="20">
+      <c r="J17" s="20">
         <v>320</v>
       </c>
-      <c r="J17" s="15">
+      <c r="K17" s="15">
         <v>70</v>
       </c>
-      <c r="K17" s="20">
+      <c r="L17" s="20">
         <v>100</v>
       </c>
-      <c r="L17" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M17" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>215</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="20">
         <v>6565</v>
       </c>
-      <c r="C18" s="20">
+      <c r="D18" s="20">
         <v>2760</v>
       </c>
-      <c r="D18" s="20">
+      <c r="E18" s="20">
         <v>1545</v>
       </c>
-      <c r="E18" s="20">
+      <c r="F18" s="20">
         <v>260</v>
       </c>
-      <c r="F18" s="20">
-        <v>0</v>
-      </c>
       <c r="G18" s="20">
+        <v>0</v>
+      </c>
+      <c r="H18" s="20">
         <v>950</v>
       </c>
-      <c r="H18" s="15">
+      <c r="I18" s="15">
         <v>80</v>
       </c>
-      <c r="I18" s="20">
+      <c r="J18" s="20">
         <v>390</v>
       </c>
-      <c r="J18" s="15">
+      <c r="K18" s="15">
         <v>125</v>
       </c>
-      <c r="K18" s="20">
+      <c r="L18" s="20">
         <v>350</v>
       </c>
-      <c r="L18" s="15">
+      <c r="M18" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>216</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="20">
         <v>5494</v>
       </c>
-      <c r="C19" s="20">
+      <c r="D19" s="20">
         <v>2205</v>
       </c>
-      <c r="D19" s="20">
+      <c r="E19" s="20">
         <v>1710</v>
       </c>
-      <c r="E19" s="20">
+      <c r="F19" s="20">
         <v>220</v>
       </c>
-      <c r="F19" s="20">
-        <v>0</v>
-      </c>
       <c r="G19" s="20">
+        <v>0</v>
+      </c>
+      <c r="H19" s="20">
         <v>275</v>
       </c>
-      <c r="H19" s="15">
+      <c r="I19" s="15">
         <v>5</v>
       </c>
-      <c r="I19" s="20">
+      <c r="J19" s="20">
         <v>55</v>
       </c>
-      <c r="J19" s="15">
+      <c r="K19" s="15">
         <v>50</v>
       </c>
-      <c r="K19" s="20">
+      <c r="L19" s="20">
         <v>170</v>
       </c>
-      <c r="L19" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M19" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>217</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="20">
         <v>5782</v>
       </c>
-      <c r="C20" s="20">
+      <c r="D20" s="20">
         <v>2760</v>
       </c>
-      <c r="D20" s="20">
+      <c r="E20" s="20">
         <v>280</v>
       </c>
-      <c r="E20" s="20">
+      <c r="F20" s="20">
         <v>270</v>
       </c>
-      <c r="F20" s="20">
-        <v>0</v>
-      </c>
       <c r="G20" s="20">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20">
         <v>2210</v>
       </c>
-      <c r="H20" s="15">
+      <c r="I20" s="15">
         <v>15</v>
       </c>
-      <c r="I20" s="20">
+      <c r="J20" s="20">
         <v>5</v>
       </c>
-      <c r="J20" s="15">
+      <c r="K20" s="15">
         <v>10</v>
       </c>
-      <c r="K20" s="20">
+      <c r="L20" s="20">
         <v>2185</v>
       </c>
-      <c r="L20" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M20" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>218</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="20">
         <v>2657</v>
       </c>
-      <c r="C21" s="20">
+      <c r="D21" s="20">
         <v>1055</v>
       </c>
-      <c r="D21" s="20">
+      <c r="E21" s="20">
         <v>880</v>
       </c>
-      <c r="E21" s="20">
+      <c r="F21" s="20">
         <v>115</v>
       </c>
-      <c r="F21" s="20">
-        <v>0</v>
-      </c>
       <c r="G21" s="20">
+        <v>0</v>
+      </c>
+      <c r="H21" s="20">
         <v>55</v>
       </c>
-      <c r="H21" s="15">
-        <v>0</v>
-      </c>
-      <c r="I21" s="20">
-        <v>0</v>
-      </c>
-      <c r="J21" s="15">
+      <c r="I21" s="15">
+        <v>0</v>
+      </c>
+      <c r="J21" s="20">
+        <v>0</v>
+      </c>
+      <c r="K21" s="15">
         <v>25</v>
       </c>
-      <c r="K21" s="20">
+      <c r="L21" s="20">
         <v>35</v>
       </c>
-      <c r="L21" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M21" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>219</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="20">
         <v>4193</v>
       </c>
-      <c r="C22" s="20">
+      <c r="D22" s="20">
         <v>1640</v>
       </c>
-      <c r="D22" s="20">
+      <c r="E22" s="20">
         <v>1460</v>
       </c>
-      <c r="E22" s="20">
+      <c r="F22" s="20">
         <v>110</v>
       </c>
-      <c r="F22" s="20">
-        <v>0</v>
-      </c>
       <c r="G22" s="20">
+        <v>0</v>
+      </c>
+      <c r="H22" s="20">
         <v>65</v>
       </c>
-      <c r="H22" s="15">
-        <v>0</v>
-      </c>
-      <c r="I22" s="20">
+      <c r="I22" s="15">
+        <v>0</v>
+      </c>
+      <c r="J22" s="20">
         <v>5</v>
       </c>
-      <c r="J22" s="15">
+      <c r="K22" s="15">
         <v>45</v>
       </c>
-      <c r="K22" s="20">
+      <c r="L22" s="20">
         <v>20</v>
       </c>
-      <c r="L22" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M22" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>220</v>
       </c>
-      <c r="B23" s="20">
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="20">
         <v>4069</v>
       </c>
-      <c r="C23" s="20">
+      <c r="D23" s="20">
         <v>1585</v>
       </c>
-      <c r="D23" s="20">
+      <c r="E23" s="20">
         <v>790</v>
       </c>
-      <c r="E23" s="20">
+      <c r="F23" s="20">
         <v>525</v>
       </c>
-      <c r="F23" s="20">
-        <v>0</v>
-      </c>
       <c r="G23" s="20">
+        <v>0</v>
+      </c>
+      <c r="H23" s="20">
         <v>265</v>
       </c>
-      <c r="H23" s="15">
+      <c r="I23" s="15">
         <v>5</v>
       </c>
-      <c r="I23" s="20">
+      <c r="J23" s="20">
         <v>80</v>
       </c>
-      <c r="J23" s="15">
+      <c r="K23" s="15">
         <v>45</v>
       </c>
-      <c r="K23" s="20">
+      <c r="L23" s="20">
         <v>135</v>
       </c>
-      <c r="L23" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M23" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
         <v>221</v>
       </c>
-      <c r="F24" s="20"/>
-    </row>
-    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>221.01</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="20">
         <v>6367</v>
       </c>
-      <c r="C25" s="20">
+      <c r="D25" s="20">
         <v>2725</v>
       </c>
-      <c r="D25" s="20">
+      <c r="E25" s="20">
         <v>1005</v>
       </c>
-      <c r="E25" s="20">
+      <c r="F25" s="20">
         <v>1490</v>
       </c>
-      <c r="F25" s="20">
-        <v>0</v>
-      </c>
       <c r="G25" s="20">
+        <v>0</v>
+      </c>
+      <c r="H25" s="20">
         <v>225</v>
       </c>
-      <c r="H25" s="15">
-        <v>0</v>
-      </c>
-      <c r="I25" s="20">
+      <c r="I25" s="15">
+        <v>0</v>
+      </c>
+      <c r="J25" s="20">
         <v>205</v>
       </c>
-      <c r="J25" s="15">
+      <c r="K25" s="15">
         <v>15</v>
       </c>
-      <c r="K25" s="20">
-        <v>0</v>
-      </c>
-      <c r="L25" s="15">
+      <c r="L25" s="20">
+        <v>0</v>
+      </c>
+      <c r="M25" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>221.02</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="20">
         <v>4376</v>
       </c>
-      <c r="C26" s="20">
+      <c r="D26" s="20">
         <v>1565</v>
       </c>
-      <c r="D26" s="20">
+      <c r="E26" s="20">
         <v>445</v>
       </c>
-      <c r="E26" s="20">
+      <c r="F26" s="20">
         <v>1055</v>
       </c>
-      <c r="F26" s="20">
-        <v>0</v>
-      </c>
       <c r="G26" s="20">
+        <v>0</v>
+      </c>
+      <c r="H26" s="20">
         <v>70</v>
       </c>
-      <c r="H26" s="15">
-        <v>0</v>
-      </c>
-      <c r="I26" s="20">
-        <v>0</v>
-      </c>
-      <c r="J26" s="15">
+      <c r="I26" s="15">
+        <v>0</v>
+      </c>
+      <c r="J26" s="20">
+        <v>0</v>
+      </c>
+      <c r="K26" s="15">
         <v>15</v>
       </c>
-      <c r="K26" s="20">
+      <c r="L26" s="20">
         <v>55</v>
       </c>
-      <c r="L26" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="M26" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>222.01</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="20">
         <v>5409</v>
       </c>
-      <c r="C27" s="20">
+      <c r="D27" s="20">
         <v>1935</v>
       </c>
-      <c r="D27" s="20">
+      <c r="E27" s="20">
         <v>920</v>
       </c>
-      <c r="E27" s="20">
+      <c r="F27" s="20">
         <v>400</v>
       </c>
-      <c r="F27" s="20">
-        <v>0</v>
-      </c>
       <c r="G27" s="20">
+        <v>0</v>
+      </c>
+      <c r="H27" s="20">
         <v>610</v>
       </c>
-      <c r="H27" s="15">
+      <c r="I27" s="15">
         <v>20</v>
       </c>
-      <c r="I27" s="20">
+      <c r="J27" s="20">
         <v>115</v>
       </c>
-      <c r="J27" s="15">
+      <c r="K27" s="15">
         <v>45</v>
       </c>
-      <c r="K27" s="20">
+      <c r="L27" s="20">
         <v>430</v>
       </c>
-      <c r="L27" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="M27" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>222.02</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="20">
         <v>5124</v>
       </c>
-      <c r="C28" s="20">
+      <c r="D28" s="20">
         <v>1795</v>
       </c>
-      <c r="D28" s="20">
+      <c r="E28" s="20">
         <v>810</v>
       </c>
-      <c r="E28" s="20">
+      <c r="F28" s="20">
         <v>940</v>
       </c>
-      <c r="F28" s="20">
-        <v>0</v>
-      </c>
       <c r="G28" s="20">
+        <v>0</v>
+      </c>
+      <c r="H28" s="20">
         <v>50</v>
       </c>
-      <c r="H28" s="16">
+      <c r="I28" s="16">
         <v>25</v>
       </c>
-      <c r="I28" s="20">
-        <v>0</v>
-      </c>
-      <c r="J28" s="16">
+      <c r="J28" s="20">
+        <v>0</v>
+      </c>
+      <c r="K28" s="16">
         <v>20</v>
       </c>
-      <c r="K28" s="20">
-        <v>0</v>
-      </c>
-      <c r="L28" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L28" s="20">
+        <v>0</v>
+      </c>
+      <c r="M28" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>223</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="20">
         <v>3641</v>
       </c>
-      <c r="C29" s="20">
+      <c r="D29" s="20">
         <v>1285</v>
       </c>
-      <c r="D29" s="20">
+      <c r="E29" s="20">
         <v>1175</v>
       </c>
-      <c r="E29" s="20">
-        <v>0</v>
-      </c>
       <c r="F29" s="20">
         <v>0</v>
       </c>
       <c r="G29" s="20">
+        <v>0</v>
+      </c>
+      <c r="H29" s="20">
         <v>110</v>
       </c>
-      <c r="H29" s="16">
-        <v>0</v>
-      </c>
-      <c r="I29" s="20">
+      <c r="I29" s="16">
+        <v>0</v>
+      </c>
+      <c r="J29" s="20">
         <v>10</v>
       </c>
-      <c r="J29" s="16">
+      <c r="K29" s="16">
         <v>40</v>
       </c>
-      <c r="K29" s="20">
+      <c r="L29" s="20">
         <v>55</v>
       </c>
-      <c r="L29" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M29" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>224</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="20">
         <v>1743</v>
       </c>
-      <c r="C30" s="20">
+      <c r="D30" s="20">
         <v>580</v>
       </c>
-      <c r="D30" s="20">
+      <c r="E30" s="20">
         <v>565</v>
       </c>
-      <c r="E30" s="20">
-        <v>0</v>
-      </c>
       <c r="F30" s="20">
         <v>0</v>
       </c>
       <c r="G30" s="20">
+        <v>0</v>
+      </c>
+      <c r="H30" s="20">
         <v>15</v>
       </c>
-      <c r="H30" s="15">
-        <v>0</v>
-      </c>
-      <c r="I30" s="20">
-        <v>0</v>
-      </c>
-      <c r="J30" s="15">
+      <c r="I30" s="15">
+        <v>0</v>
+      </c>
+      <c r="J30" s="20">
+        <v>0</v>
+      </c>
+      <c r="K30" s="15">
         <v>15</v>
       </c>
-      <c r="K30" s="20">
-        <v>0</v>
-      </c>
-      <c r="L30" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L30" s="20">
+        <v>0</v>
+      </c>
+      <c r="M30" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>225.01</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="20">
         <v>5034</v>
       </c>
-      <c r="C31" s="20">
+      <c r="D31" s="20">
         <v>2345</v>
       </c>
-      <c r="D31" s="20">
+      <c r="E31" s="20">
         <v>470</v>
       </c>
-      <c r="E31" s="20">
+      <c r="F31" s="20">
         <v>1690</v>
       </c>
-      <c r="F31" s="20">
-        <v>0</v>
-      </c>
       <c r="G31" s="20">
+        <v>0</v>
+      </c>
+      <c r="H31" s="20">
         <v>185</v>
       </c>
-      <c r="H31" s="15">
+      <c r="I31" s="15">
         <v>15</v>
       </c>
-      <c r="I31" s="20">
+      <c r="J31" s="20">
         <v>45</v>
       </c>
-      <c r="J31" s="15">
+      <c r="K31" s="15">
         <v>10</v>
       </c>
-      <c r="K31" s="20">
+      <c r="L31" s="20">
         <v>115</v>
       </c>
-      <c r="L31" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M31" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>225.02</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="20">
         <v>7777</v>
       </c>
-      <c r="C32" s="20">
+      <c r="D32" s="20">
         <v>3755</v>
       </c>
-      <c r="D32" s="20">
-        <v>0</v>
-      </c>
       <c r="E32" s="20">
+        <v>0</v>
+      </c>
+      <c r="F32" s="20">
         <v>3680</v>
       </c>
-      <c r="F32" s="20">
-        <v>0</v>
-      </c>
       <c r="G32" s="20">
+        <v>0</v>
+      </c>
+      <c r="H32" s="20">
         <v>75</v>
       </c>
-      <c r="H32" s="15">
-        <v>0</v>
-      </c>
-      <c r="I32" s="20">
+      <c r="I32" s="15">
+        <v>0</v>
+      </c>
+      <c r="J32" s="20">
         <v>65</v>
       </c>
-      <c r="J32" s="15">
-        <v>0</v>
-      </c>
-      <c r="K32" s="20">
+      <c r="K32" s="15">
+        <v>0</v>
+      </c>
+      <c r="L32" s="20">
         <v>10</v>
       </c>
-      <c r="L32" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M32" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>226</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="20">
         <v>3216</v>
       </c>
-      <c r="C33" s="20">
+      <c r="D33" s="20">
         <v>1260</v>
       </c>
-      <c r="D33" s="20">
+      <c r="E33" s="20">
         <v>930</v>
       </c>
-      <c r="E33" s="20">
+      <c r="F33" s="20">
         <v>210</v>
       </c>
-      <c r="F33" s="20">
-        <v>0</v>
-      </c>
       <c r="G33" s="20">
+        <v>0</v>
+      </c>
+      <c r="H33" s="20">
         <v>115</v>
       </c>
-      <c r="H33" s="15">
+      <c r="I33" s="15">
         <v>65</v>
       </c>
-      <c r="I33" s="20">
+      <c r="J33" s="20">
         <v>5</v>
       </c>
-      <c r="J33" s="15">
+      <c r="K33" s="15">
         <v>10</v>
       </c>
-      <c r="K33" s="20">
+      <c r="L33" s="20">
         <v>35</v>
       </c>
-      <c r="L33" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M33" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>227</v>
       </c>
-      <c r="B34" s="20">
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" s="20">
         <v>1748</v>
       </c>
-      <c r="C34" s="20">
+      <c r="D34" s="20">
         <v>620</v>
       </c>
-      <c r="D34" s="20">
+      <c r="E34" s="20">
         <v>535</v>
       </c>
-      <c r="E34" s="20">
-        <v>0</v>
-      </c>
       <c r="F34" s="20">
         <v>0</v>
       </c>
       <c r="G34" s="20">
+        <v>0</v>
+      </c>
+      <c r="H34" s="20">
         <v>80</v>
       </c>
-      <c r="H34" s="15">
-        <v>0</v>
-      </c>
-      <c r="I34" s="20">
-        <v>0</v>
-      </c>
-      <c r="J34" s="15">
-        <v>0</v>
-      </c>
-      <c r="K34" s="20">
+      <c r="I34" s="15">
+        <v>0</v>
+      </c>
+      <c r="J34" s="20">
+        <v>0</v>
+      </c>
+      <c r="K34" s="15">
+        <v>0</v>
+      </c>
+      <c r="L34" s="20">
         <v>75</v>
       </c>
-      <c r="L34" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M34" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>228</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="20">
         <v>2951</v>
       </c>
-      <c r="C35" s="20">
+      <c r="D35" s="20">
         <v>1260</v>
       </c>
-      <c r="D35" s="20">
+      <c r="E35" s="20">
         <v>520</v>
       </c>
-      <c r="E35" s="20">
+      <c r="F35" s="20">
         <v>485</v>
       </c>
-      <c r="F35" s="20">
-        <v>0</v>
-      </c>
       <c r="G35" s="20">
+        <v>0</v>
+      </c>
+      <c r="H35" s="20">
         <v>255</v>
       </c>
-      <c r="H35" s="15">
+      <c r="I35" s="15">
         <v>5</v>
       </c>
-      <c r="I35" s="20">
+      <c r="J35" s="20">
         <v>45</v>
       </c>
-      <c r="J35" s="15">
+      <c r="K35" s="15">
         <v>5</v>
       </c>
-      <c r="K35" s="20">
+      <c r="L35" s="20">
         <v>205</v>
       </c>
-      <c r="L35" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M35" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>229</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="20">
         <v>1255</v>
       </c>
-      <c r="C36" s="20">
+      <c r="D36" s="20">
         <v>390</v>
       </c>
-      <c r="D36" s="20">
+      <c r="E36" s="20">
         <v>365</v>
       </c>
-      <c r="E36" s="20">
-        <v>0</v>
-      </c>
       <c r="F36" s="20">
         <v>0</v>
       </c>
       <c r="G36" s="20">
+        <v>0</v>
+      </c>
+      <c r="H36" s="20">
         <v>30</v>
       </c>
-      <c r="H36" s="15">
-        <v>0</v>
-      </c>
-      <c r="I36" s="20">
-        <v>0</v>
-      </c>
-      <c r="J36" s="15">
+      <c r="I36" s="15">
+        <v>0</v>
+      </c>
+      <c r="J36" s="20">
+        <v>0</v>
+      </c>
+      <c r="K36" s="15">
         <v>10</v>
       </c>
-      <c r="K36" s="20">
+      <c r="L36" s="20">
         <v>20</v>
       </c>
-      <c r="L36" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M36" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>230.01</v>
       </c>
-      <c r="B37" s="20">
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="20">
         <v>2279</v>
       </c>
-      <c r="C37" s="20">
+      <c r="D37" s="20">
         <v>990</v>
       </c>
-      <c r="D37" s="20">
+      <c r="E37" s="20">
         <v>425</v>
       </c>
-      <c r="E37" s="20">
+      <c r="F37" s="20">
         <v>500</v>
       </c>
-      <c r="F37" s="20">
-        <v>0</v>
-      </c>
       <c r="G37" s="20">
+        <v>0</v>
+      </c>
+      <c r="H37" s="20">
         <v>70</v>
       </c>
-      <c r="H37" s="15">
-        <v>0</v>
-      </c>
-      <c r="I37" s="20">
+      <c r="I37" s="15">
+        <v>0</v>
+      </c>
+      <c r="J37" s="20">
         <v>5</v>
       </c>
-      <c r="J37" s="15">
+      <c r="K37" s="15">
         <v>10</v>
       </c>
-      <c r="K37" s="20">
+      <c r="L37" s="20">
         <v>50</v>
       </c>
-      <c r="L37" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M37" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
         <v>230.02</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="20">
         <v>6176</v>
       </c>
-      <c r="C38" s="20">
+      <c r="D38" s="20">
         <v>2455</v>
       </c>
-      <c r="D38" s="20">
+      <c r="E38" s="20">
         <v>560</v>
       </c>
-      <c r="E38" s="20">
+      <c r="F38" s="20">
         <v>1605</v>
       </c>
-      <c r="F38" s="20">
-        <v>0</v>
-      </c>
       <c r="G38" s="20">
+        <v>0</v>
+      </c>
+      <c r="H38" s="20">
         <v>285</v>
       </c>
-      <c r="H38" s="15">
+      <c r="I38" s="15">
         <v>90</v>
       </c>
-      <c r="I38" s="20">
+      <c r="J38" s="20">
         <v>115</v>
       </c>
-      <c r="J38" s="15">
+      <c r="K38" s="15">
         <v>15</v>
       </c>
-      <c r="K38" s="20">
+      <c r="L38" s="20">
         <v>70</v>
       </c>
-      <c r="L38" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M38" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
         <v>231</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="20">
         <v>6488</v>
       </c>
-      <c r="C39" s="20">
+      <c r="D39" s="20">
         <v>2580</v>
       </c>
-      <c r="D39" s="20">
+      <c r="E39" s="20">
         <v>1580</v>
       </c>
-      <c r="E39" s="20">
+      <c r="F39" s="20">
         <v>65</v>
       </c>
-      <c r="F39" s="20">
-        <v>0</v>
-      </c>
       <c r="G39" s="20">
+        <v>0</v>
+      </c>
+      <c r="H39" s="20">
         <v>930</v>
       </c>
-      <c r="H39" s="15">
+      <c r="I39" s="15">
         <v>5</v>
       </c>
-      <c r="I39" s="20">
-        <v>0</v>
-      </c>
-      <c r="J39" s="15">
+      <c r="J39" s="20">
+        <v>0</v>
+      </c>
+      <c r="K39" s="15">
         <v>20</v>
       </c>
-      <c r="K39" s="20">
+      <c r="L39" s="20">
         <v>905</v>
       </c>
-      <c r="L39" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M39" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <v>232</v>
       </c>
-      <c r="B40" s="20">
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="20">
         <v>3995</v>
       </c>
-      <c r="C40" s="20">
+      <c r="D40" s="20">
         <v>1320</v>
       </c>
-      <c r="D40" s="20">
+      <c r="E40" s="20">
         <v>1250</v>
       </c>
-      <c r="E40" s="20">
-        <v>0</v>
-      </c>
       <c r="F40" s="20">
         <v>0</v>
       </c>
       <c r="G40" s="20">
+        <v>0</v>
+      </c>
+      <c r="H40" s="20">
         <v>65</v>
       </c>
-      <c r="H40" s="15">
-        <v>0</v>
-      </c>
-      <c r="I40" s="20">
+      <c r="I40" s="15">
+        <v>0</v>
+      </c>
+      <c r="J40" s="20">
         <v>40</v>
       </c>
-      <c r="J40" s="15">
+      <c r="K40" s="15">
         <v>15</v>
       </c>
-      <c r="K40" s="20">
+      <c r="L40" s="20">
         <v>15</v>
       </c>
-      <c r="L40" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M40" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <v>233</v>
       </c>
-      <c r="B41" s="20">
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" s="20">
         <v>5459</v>
       </c>
-      <c r="C41" s="20">
+      <c r="D41" s="20">
         <v>1965</v>
       </c>
-      <c r="D41" s="20">
+      <c r="E41" s="20">
         <v>1490</v>
       </c>
-      <c r="E41" s="20">
+      <c r="F41" s="20">
         <v>445</v>
       </c>
-      <c r="F41" s="20">
-        <v>0</v>
-      </c>
       <c r="G41" s="20">
+        <v>0</v>
+      </c>
+      <c r="H41" s="20">
         <v>25</v>
       </c>
-      <c r="H41" s="15">
-        <v>0</v>
-      </c>
-      <c r="I41" s="20">
-        <v>0</v>
-      </c>
-      <c r="J41" s="15">
+      <c r="I41" s="15">
+        <v>0</v>
+      </c>
+      <c r="J41" s="20">
+        <v>0</v>
+      </c>
+      <c r="K41" s="15">
         <v>25</v>
       </c>
-      <c r="K41" s="20">
-        <v>0</v>
-      </c>
-      <c r="L41" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L41" s="20">
+        <v>0</v>
+      </c>
+      <c r="M41" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <v>234</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="20">
         <v>4550</v>
       </c>
-      <c r="C42" s="20">
+      <c r="D42" s="20">
         <v>1630</v>
       </c>
-      <c r="D42" s="20">
+      <c r="E42" s="20">
         <v>1270</v>
       </c>
-      <c r="E42" s="20">
+      <c r="F42" s="20">
         <v>35</v>
       </c>
-      <c r="F42" s="20">
-        <v>0</v>
-      </c>
       <c r="G42" s="20">
+        <v>0</v>
+      </c>
+      <c r="H42" s="20">
         <v>320</v>
       </c>
-      <c r="H42" s="15">
-        <v>0</v>
-      </c>
-      <c r="I42" s="20">
+      <c r="I42" s="15">
+        <v>0</v>
+      </c>
+      <c r="J42" s="20">
         <v>215</v>
       </c>
-      <c r="J42" s="15">
+      <c r="K42" s="15">
         <v>40</v>
       </c>
-      <c r="K42" s="20">
+      <c r="L42" s="20">
         <v>65</v>
       </c>
-      <c r="L42" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M42" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
         <v>235.01</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" s="20">
         <v>2812</v>
       </c>
-      <c r="C43" s="20">
+      <c r="D43" s="20">
         <v>1000</v>
       </c>
-      <c r="D43" s="20">
+      <c r="E43" s="20">
         <v>890</v>
       </c>
-      <c r="E43" s="20">
-        <v>0</v>
-      </c>
       <c r="F43" s="20">
         <v>0</v>
       </c>
       <c r="G43" s="20">
+        <v>0</v>
+      </c>
+      <c r="H43" s="20">
         <v>110</v>
       </c>
-      <c r="H43" s="15">
+      <c r="I43" s="15">
         <v>35</v>
       </c>
-      <c r="I43" s="20">
+      <c r="J43" s="20">
         <v>35</v>
       </c>
-      <c r="J43" s="15">
+      <c r="K43" s="15">
         <v>35</v>
       </c>
-      <c r="K43" s="20">
-        <v>0</v>
-      </c>
-      <c r="L43" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L43" s="20">
+        <v>0</v>
+      </c>
+      <c r="M43" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>235.02</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" s="20">
         <v>5397</v>
       </c>
-      <c r="C44" s="20">
+      <c r="D44" s="20">
         <v>2030</v>
       </c>
-      <c r="D44" s="20">
+      <c r="E44" s="20">
         <v>815</v>
       </c>
-      <c r="E44" s="20">
+      <c r="F44" s="20">
         <v>1090</v>
       </c>
-      <c r="F44" s="20">
-        <v>0</v>
-      </c>
       <c r="G44" s="20">
+        <v>0</v>
+      </c>
+      <c r="H44" s="20">
         <v>125</v>
       </c>
-      <c r="H44" s="15">
+      <c r="I44" s="15">
         <v>90</v>
       </c>
-      <c r="I44" s="20">
-        <v>0</v>
-      </c>
-      <c r="J44" s="15">
+      <c r="J44" s="20">
+        <v>0</v>
+      </c>
+      <c r="K44" s="15">
         <v>30</v>
       </c>
-      <c r="K44" s="20">
-        <v>0</v>
-      </c>
-      <c r="L44" s="15">
+      <c r="L44" s="20">
+        <v>0</v>
+      </c>
+      <c r="M44" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
         <v>236.01</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" s="20">
         <v>6551</v>
       </c>
-      <c r="C45" s="20">
+      <c r="D45" s="20">
         <v>2535</v>
       </c>
-      <c r="D45" s="20">
+      <c r="E45" s="20">
         <v>555</v>
       </c>
-      <c r="E45" s="20">
+      <c r="F45" s="20">
         <v>1620</v>
       </c>
-      <c r="F45" s="20">
-        <v>0</v>
-      </c>
       <c r="G45" s="20">
+        <v>0</v>
+      </c>
+      <c r="H45" s="20">
         <v>360</v>
       </c>
-      <c r="H45" s="15">
+      <c r="I45" s="15">
         <v>95</v>
       </c>
-      <c r="I45" s="20">
+      <c r="J45" s="20">
         <v>220</v>
       </c>
-      <c r="J45" s="15">
+      <c r="K45" s="15">
         <v>35</v>
       </c>
-      <c r="K45" s="20">
-        <v>0</v>
-      </c>
-      <c r="L45" s="15">
+      <c r="L45" s="20">
+        <v>0</v>
+      </c>
+      <c r="M45" s="15">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>236.02</v>
       </c>
-      <c r="B46" s="20">
+      <c r="B46" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46" s="20">
         <v>6051</v>
       </c>
-      <c r="C46" s="20">
+      <c r="D46" s="20">
         <v>2240</v>
       </c>
-      <c r="D46" s="20">
+      <c r="E46" s="20">
         <v>985</v>
       </c>
-      <c r="E46" s="20">
+      <c r="F46" s="20">
         <v>665</v>
       </c>
-      <c r="F46" s="20">
-        <v>0</v>
-      </c>
       <c r="G46" s="20">
+        <v>0</v>
+      </c>
+      <c r="H46" s="20">
         <v>590</v>
       </c>
-      <c r="H46" s="15">
+      <c r="I46" s="15">
         <v>225</v>
       </c>
-      <c r="I46" s="20">
+      <c r="J46" s="20">
         <v>350</v>
       </c>
-      <c r="J46" s="15">
+      <c r="K46" s="15">
         <v>10</v>
       </c>
-      <c r="K46" s="20">
-        <v>0</v>
-      </c>
-      <c r="L46" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L46" s="20">
+        <v>0</v>
+      </c>
+      <c r="M46" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>237.01</v>
       </c>
-      <c r="B47" s="20">
+      <c r="B47" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" s="20">
         <v>6258</v>
       </c>
-      <c r="C47" s="20">
+      <c r="D47" s="20">
         <v>2150</v>
       </c>
-      <c r="D47" s="20">
+      <c r="E47" s="20">
         <v>325</v>
       </c>
-      <c r="E47" s="20">
+      <c r="F47" s="20">
         <v>1290</v>
       </c>
-      <c r="F47" s="20">
-        <v>0</v>
-      </c>
       <c r="G47" s="20">
+        <v>0</v>
+      </c>
+      <c r="H47" s="20">
         <v>530</v>
       </c>
-      <c r="H47" s="15">
+      <c r="I47" s="15">
         <v>450</v>
       </c>
-      <c r="I47" s="20">
-        <v>0</v>
-      </c>
-      <c r="J47" s="15">
+      <c r="J47" s="20">
+        <v>0</v>
+      </c>
+      <c r="K47" s="15">
         <v>75</v>
       </c>
-      <c r="K47" s="20">
+      <c r="L47" s="20">
         <v>10</v>
       </c>
-      <c r="L47" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M47" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>237.02</v>
       </c>
-      <c r="B48" s="20">
+      <c r="B48" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" s="20">
         <v>2861</v>
       </c>
-      <c r="C48" s="20">
+      <c r="D48" s="20">
         <v>1055</v>
       </c>
-      <c r="D48" s="20">
+      <c r="E48" s="20">
         <v>835</v>
       </c>
-      <c r="E48" s="20">
+      <c r="F48" s="20">
         <v>105</v>
       </c>
-      <c r="F48" s="20">
-        <v>0</v>
-      </c>
       <c r="G48" s="20">
+        <v>0</v>
+      </c>
+      <c r="H48" s="20">
         <v>120</v>
       </c>
-      <c r="H48" s="15">
-        <v>0</v>
-      </c>
-      <c r="I48" s="20">
+      <c r="I48" s="15">
+        <v>0</v>
+      </c>
+      <c r="J48" s="20">
         <v>35</v>
       </c>
-      <c r="J48" s="15">
+      <c r="K48" s="15">
         <v>75</v>
       </c>
-      <c r="K48" s="20">
+      <c r="L48" s="20">
         <v>15</v>
       </c>
-      <c r="L48" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M48" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>237.03</v>
       </c>
-      <c r="B49" s="20">
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" s="20">
         <v>5522</v>
       </c>
-      <c r="C49" s="20">
+      <c r="D49" s="20">
         <v>2425</v>
       </c>
-      <c r="D49" s="20">
+      <c r="E49" s="20">
         <v>435</v>
       </c>
-      <c r="E49" s="20">
+      <c r="F49" s="20">
         <v>1760</v>
       </c>
-      <c r="F49" s="20">
-        <v>0</v>
-      </c>
       <c r="G49" s="20">
+        <v>0</v>
+      </c>
+      <c r="H49" s="20">
         <v>230</v>
       </c>
-      <c r="H49" s="15">
+      <c r="I49" s="15">
         <v>90</v>
       </c>
-      <c r="I49" s="20">
+      <c r="J49" s="20">
         <v>110</v>
       </c>
-      <c r="J49" s="15">
+      <c r="K49" s="15">
         <v>30</v>
       </c>
-      <c r="K49" s="20">
-        <v>0</v>
-      </c>
-      <c r="L49" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L49" s="20">
+        <v>0</v>
+      </c>
+      <c r="M49" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>238.01</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50" s="20">
         <v>3336</v>
       </c>
-      <c r="C50" s="20">
+      <c r="D50" s="20">
         <v>1250</v>
       </c>
-      <c r="D50" s="20">
+      <c r="E50" s="20">
         <v>885</v>
       </c>
-      <c r="E50" s="20">
+      <c r="F50" s="20">
         <v>265</v>
       </c>
-      <c r="F50" s="20">
-        <v>0</v>
-      </c>
       <c r="G50" s="20">
+        <v>0</v>
+      </c>
+      <c r="H50" s="20">
         <v>100</v>
       </c>
-      <c r="H50" s="15">
-        <v>0</v>
-      </c>
-      <c r="I50" s="20">
+      <c r="I50" s="15">
+        <v>0</v>
+      </c>
+      <c r="J50" s="20">
         <v>80</v>
       </c>
-      <c r="J50" s="15">
+      <c r="K50" s="15">
         <v>20</v>
       </c>
-      <c r="K50" s="20">
-        <v>0</v>
-      </c>
-      <c r="L50" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L50" s="20">
+        <v>0</v>
+      </c>
+      <c r="M50" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>238.02</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B51" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" s="20">
         <v>5199</v>
       </c>
-      <c r="C51" s="20">
+      <c r="D51" s="20">
         <v>1965</v>
       </c>
-      <c r="D51" s="20">
+      <c r="E51" s="20">
         <v>755</v>
       </c>
-      <c r="E51" s="20">
+      <c r="F51" s="20">
         <v>1165</v>
       </c>
-      <c r="F51" s="20">
-        <v>0</v>
-      </c>
       <c r="G51" s="20">
+        <v>0</v>
+      </c>
+      <c r="H51" s="20">
         <v>45</v>
       </c>
-      <c r="H51" s="15">
+      <c r="I51" s="15">
         <v>15</v>
       </c>
-      <c r="I51" s="20">
-        <v>0</v>
-      </c>
-      <c r="J51" s="15">
+      <c r="J51" s="20">
+        <v>0</v>
+      </c>
+      <c r="K51" s="15">
         <v>25</v>
       </c>
-      <c r="K51" s="20">
-        <v>0</v>
-      </c>
-      <c r="L51" s="15">
+      <c r="L51" s="20">
+        <v>0</v>
+      </c>
+      <c r="M51" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>239</v>
       </c>
-      <c r="B52" s="20">
+      <c r="B52" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52" s="20">
         <v>6571</v>
       </c>
-      <c r="C52" s="20">
+      <c r="D52" s="20">
         <v>2375</v>
       </c>
-      <c r="D52" s="20">
+      <c r="E52" s="20">
         <v>775</v>
       </c>
-      <c r="E52" s="20">
+      <c r="F52" s="20">
         <v>1165</v>
       </c>
-      <c r="F52" s="20">
-        <v>0</v>
-      </c>
       <c r="G52" s="20">
+        <v>0</v>
+      </c>
+      <c r="H52" s="20">
         <v>435</v>
       </c>
-      <c r="H52" s="15">
+      <c r="I52" s="15">
         <v>75</v>
       </c>
-      <c r="I52" s="20">
+      <c r="J52" s="20">
         <v>210</v>
       </c>
-      <c r="J52" s="15">
+      <c r="K52" s="15">
         <v>65</v>
       </c>
-      <c r="K52" s="20">
+      <c r="L52" s="20">
         <v>90</v>
       </c>
-      <c r="L52" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M52" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <v>240.01</v>
       </c>
-      <c r="B53" s="20">
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" s="20">
         <v>3366</v>
       </c>
-      <c r="C53" s="20">
+      <c r="D53" s="20">
         <v>1270</v>
       </c>
-      <c r="D53" s="20">
+      <c r="E53" s="20">
         <v>1160</v>
       </c>
-      <c r="E53" s="20">
-        <v>0</v>
-      </c>
       <c r="F53" s="20">
         <v>0</v>
       </c>
       <c r="G53" s="20">
+        <v>0</v>
+      </c>
+      <c r="H53" s="20">
         <v>110</v>
       </c>
-      <c r="H53" s="15">
-        <v>0</v>
-      </c>
-      <c r="I53" s="20">
+      <c r="I53" s="15">
+        <v>0</v>
+      </c>
+      <c r="J53" s="20">
         <v>55</v>
       </c>
-      <c r="J53" s="15">
+      <c r="K53" s="15">
         <v>40</v>
       </c>
-      <c r="K53" s="20">
+      <c r="L53" s="20">
         <v>10</v>
       </c>
-      <c r="L53" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M53" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
         <v>240.02</v>
       </c>
-      <c r="B54" s="20">
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" s="20">
         <v>5715</v>
       </c>
-      <c r="C54" s="20">
+      <c r="D54" s="20">
         <v>2300</v>
       </c>
-      <c r="D54" s="20">
+      <c r="E54" s="20">
         <v>540</v>
       </c>
-      <c r="E54" s="20">
+      <c r="F54" s="20">
         <v>1605</v>
       </c>
-      <c r="F54" s="20">
-        <v>0</v>
-      </c>
       <c r="G54" s="20">
+        <v>0</v>
+      </c>
+      <c r="H54" s="20">
         <v>155</v>
       </c>
-      <c r="H54" s="15">
+      <c r="I54" s="15">
         <v>60</v>
       </c>
-      <c r="I54" s="20">
+      <c r="J54" s="20">
         <v>35</v>
       </c>
-      <c r="J54" s="15">
+      <c r="K54" s="15">
         <v>50</v>
       </c>
-      <c r="K54" s="20">
+      <c r="L54" s="20">
         <v>5</v>
       </c>
-      <c r="L54" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M54" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
         <v>241</v>
       </c>
-      <c r="B55" s="20">
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="20">
         <v>3127</v>
       </c>
-      <c r="C55" s="20">
+      <c r="D55" s="20">
         <v>1010</v>
       </c>
-      <c r="D55" s="20">
+      <c r="E55" s="20">
         <v>895</v>
       </c>
-      <c r="E55" s="20">
-        <v>0</v>
-      </c>
       <c r="F55" s="20">
         <v>0</v>
       </c>
       <c r="G55" s="20">
+        <v>0</v>
+      </c>
+      <c r="H55" s="20">
         <v>120</v>
       </c>
-      <c r="H55" s="15">
-        <v>0</v>
-      </c>
-      <c r="I55" s="20">
-        <v>0</v>
-      </c>
-      <c r="J55" s="15">
+      <c r="I55" s="15">
+        <v>0</v>
+      </c>
+      <c r="J55" s="20">
+        <v>0</v>
+      </c>
+      <c r="K55" s="15">
         <v>85</v>
       </c>
-      <c r="K55" s="20">
+      <c r="L55" s="20">
         <v>30</v>
       </c>
-      <c r="L55" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M55" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
         <v>242</v>
       </c>
-      <c r="B56" s="20">
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56" s="20">
         <v>1741</v>
       </c>
-      <c r="C56" s="20">
+      <c r="D56" s="20">
         <v>600</v>
       </c>
-      <c r="D56" s="20">
+      <c r="E56" s="20">
         <v>275</v>
       </c>
-      <c r="E56" s="20">
+      <c r="F56" s="20">
         <v>220</v>
       </c>
-      <c r="F56" s="20">
-        <v>0</v>
-      </c>
       <c r="G56" s="20">
+        <v>0</v>
+      </c>
+      <c r="H56" s="20">
         <v>105</v>
       </c>
-      <c r="H56" s="15">
-        <v>0</v>
-      </c>
-      <c r="I56" s="20">
+      <c r="I56" s="15">
+        <v>0</v>
+      </c>
+      <c r="J56" s="20">
         <v>25</v>
       </c>
-      <c r="J56" s="15">
+      <c r="K56" s="15">
         <v>35</v>
       </c>
-      <c r="K56" s="20">
+      <c r="L56" s="20">
         <v>40</v>
       </c>
-      <c r="L56" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M56" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
         <v>243.01</v>
       </c>
-      <c r="B57" s="20">
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" s="20">
         <v>6457</v>
       </c>
-      <c r="C57" s="20">
+      <c r="D57" s="20">
         <v>2080</v>
       </c>
-      <c r="D57" s="20">
+      <c r="E57" s="20">
         <v>60</v>
       </c>
-      <c r="E57" s="20">
+      <c r="F57" s="20">
         <v>2010</v>
       </c>
-      <c r="F57" s="20">
-        <v>0</v>
-      </c>
       <c r="G57" s="20">
+        <v>0</v>
+      </c>
+      <c r="H57" s="20">
         <v>5</v>
       </c>
-      <c r="H57" s="15">
-        <v>0</v>
-      </c>
-      <c r="I57" s="20">
-        <v>0</v>
-      </c>
-      <c r="J57" s="15">
-        <v>0</v>
-      </c>
-      <c r="K57" s="20">
-        <v>0</v>
-      </c>
-      <c r="L57" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="I57" s="15">
+        <v>0</v>
+      </c>
+      <c r="J57" s="20">
+        <v>0</v>
+      </c>
+      <c r="K57" s="15">
+        <v>0</v>
+      </c>
+      <c r="L57" s="20">
+        <v>0</v>
+      </c>
+      <c r="M57" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
         <v>243.02</v>
       </c>
-      <c r="B58" s="20">
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" s="20">
         <v>3496</v>
       </c>
-      <c r="C58" s="20">
+      <c r="D58" s="20">
         <v>1245</v>
       </c>
-      <c r="D58" s="20">
+      <c r="E58" s="20">
         <v>585</v>
       </c>
-      <c r="E58" s="20">
+      <c r="F58" s="20">
         <v>325</v>
       </c>
-      <c r="F58" s="20">
-        <v>0</v>
-      </c>
       <c r="G58" s="20">
+        <v>0</v>
+      </c>
+      <c r="H58" s="20">
         <v>335</v>
       </c>
-      <c r="H58" s="15">
+      <c r="I58" s="15">
         <v>35</v>
       </c>
-      <c r="I58" s="20">
+      <c r="J58" s="20">
         <v>100</v>
       </c>
-      <c r="J58" s="15">
+      <c r="K58" s="15">
         <v>80</v>
       </c>
-      <c r="K58" s="20">
+      <c r="L58" s="20">
         <v>120</v>
       </c>
-      <c r="L58" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M58" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
         <v>244.01</v>
       </c>
-      <c r="B59" s="20">
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59" s="20">
         <v>5795</v>
       </c>
-      <c r="C59" s="20">
+      <c r="D59" s="20">
         <v>1950</v>
       </c>
-      <c r="D59" s="20">
+      <c r="E59" s="20">
         <v>760</v>
       </c>
-      <c r="E59" s="20">
+      <c r="F59" s="20">
         <v>815</v>
       </c>
-      <c r="F59" s="20">
-        <v>0</v>
-      </c>
       <c r="G59" s="20">
+        <v>0</v>
+      </c>
+      <c r="H59" s="20">
         <v>370</v>
       </c>
-      <c r="H59" s="15">
+      <c r="I59" s="15">
         <v>70</v>
       </c>
-      <c r="I59" s="20">
+      <c r="J59" s="20">
         <v>130</v>
       </c>
-      <c r="J59" s="15">
+      <c r="K59" s="15">
         <v>120</v>
       </c>
-      <c r="K59" s="20">
+      <c r="L59" s="20">
         <v>50</v>
       </c>
-      <c r="L59" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M59" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
         <v>244.02</v>
       </c>
-      <c r="B60" s="20">
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60" s="20">
         <v>3755</v>
       </c>
-      <c r="C60" s="20">
+      <c r="D60" s="20">
         <v>1240</v>
       </c>
-      <c r="D60" s="20">
+      <c r="E60" s="20">
         <v>240</v>
       </c>
-      <c r="E60" s="20">
+      <c r="F60" s="20">
         <v>550</v>
       </c>
-      <c r="F60" s="20">
-        <v>0</v>
-      </c>
       <c r="G60" s="20">
+        <v>0</v>
+      </c>
+      <c r="H60" s="20">
         <v>450</v>
       </c>
-      <c r="H60" s="15">
-        <v>0</v>
-      </c>
-      <c r="I60" s="20">
+      <c r="I60" s="15">
+        <v>0</v>
+      </c>
+      <c r="J60" s="20">
         <v>380</v>
       </c>
-      <c r="J60" s="15">
+      <c r="K60" s="15">
         <v>60</v>
       </c>
-      <c r="K60" s="20">
+      <c r="L60" s="20">
         <v>10</v>
       </c>
-      <c r="L60" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M60" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
         <v>245</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B61" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61" s="20">
         <v>6903</v>
       </c>
-      <c r="C61" s="20">
+      <c r="D61" s="20">
         <v>2685</v>
       </c>
-      <c r="D61" s="20">
+      <c r="E61" s="20">
         <v>1065</v>
       </c>
-      <c r="E61" s="20">
+      <c r="F61" s="20">
         <v>600</v>
       </c>
-      <c r="F61" s="20">
-        <v>0</v>
-      </c>
       <c r="G61" s="20">
+        <v>0</v>
+      </c>
+      <c r="H61" s="20">
         <v>1015</v>
       </c>
-      <c r="H61" s="15">
+      <c r="I61" s="15">
         <v>15</v>
       </c>
-      <c r="I61" s="20">
+      <c r="J61" s="20">
         <v>190</v>
       </c>
-      <c r="J61" s="15">
+      <c r="K61" s="15">
         <v>235</v>
       </c>
-      <c r="K61" s="20">
+      <c r="L61" s="20">
         <v>575</v>
       </c>
-      <c r="L61" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M61" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
         <v>246</v>
       </c>
-      <c r="B62" s="20">
+      <c r="B62" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" s="20">
         <v>3585</v>
       </c>
-      <c r="C62" s="20">
+      <c r="D62" s="20">
         <v>1270</v>
       </c>
-      <c r="D62" s="20">
+      <c r="E62" s="20">
         <v>775</v>
       </c>
-      <c r="E62" s="20">
+      <c r="F62" s="20">
         <v>35</v>
       </c>
-      <c r="F62" s="20">
-        <v>0</v>
-      </c>
       <c r="G62" s="20">
+        <v>0</v>
+      </c>
+      <c r="H62" s="20">
         <v>460</v>
       </c>
-      <c r="H62" s="15">
+      <c r="I62" s="15">
         <v>15</v>
       </c>
-      <c r="I62" s="20">
+      <c r="J62" s="20">
         <v>245</v>
       </c>
-      <c r="J62" s="15">
+      <c r="K62" s="15">
         <v>135</v>
       </c>
-      <c r="K62" s="20">
+      <c r="L62" s="20">
         <v>65</v>
       </c>
-      <c r="L62" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M62" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
         <v>247.01</v>
       </c>
-      <c r="B63" s="20">
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" s="20">
         <v>8842</v>
       </c>
-      <c r="C63" s="20">
+      <c r="D63" s="20">
         <v>2590</v>
       </c>
-      <c r="D63" s="20">
+      <c r="E63" s="20">
         <v>525</v>
       </c>
-      <c r="E63" s="20">
+      <c r="F63" s="20">
         <v>1150</v>
       </c>
-      <c r="F63" s="20">
-        <v>0</v>
-      </c>
       <c r="G63" s="20">
+        <v>0</v>
+      </c>
+      <c r="H63" s="20">
         <v>910</v>
       </c>
-      <c r="H63" s="15">
+      <c r="I63" s="15">
         <v>40</v>
       </c>
-      <c r="I63" s="20">
+      <c r="J63" s="20">
         <v>320</v>
       </c>
-      <c r="J63" s="15">
+      <c r="K63" s="15">
         <v>495</v>
       </c>
-      <c r="K63" s="20">
+      <c r="L63" s="20">
         <v>55</v>
       </c>
-      <c r="L63" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M63" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
         <v>247.02</v>
       </c>
-      <c r="B64" s="20">
+      <c r="B64" t="b">
+        <v>0</v>
+      </c>
+      <c r="C64" s="20">
         <v>6864</v>
       </c>
-      <c r="C64" s="20">
+      <c r="D64" s="20">
         <v>2220</v>
       </c>
-      <c r="D64" s="20">
+      <c r="E64" s="20">
         <v>1560</v>
       </c>
-      <c r="E64" s="20">
+      <c r="F64" s="20">
         <v>195</v>
       </c>
-      <c r="F64" s="20">
-        <v>0</v>
-      </c>
       <c r="G64" s="20">
+        <v>0</v>
+      </c>
+      <c r="H64" s="20">
         <v>470</v>
       </c>
-      <c r="H64" s="15">
+      <c r="I64" s="15">
         <v>5</v>
       </c>
-      <c r="I64" s="20">
-        <v>0</v>
-      </c>
-      <c r="J64" s="15">
+      <c r="J64" s="20">
+        <v>0</v>
+      </c>
+      <c r="K64" s="15">
         <v>280</v>
       </c>
-      <c r="K64" s="20">
+      <c r="L64" s="20">
         <v>185</v>
       </c>
-      <c r="L64" s="15">
+      <c r="M64" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="19">
         <v>248.01</v>
       </c>
-      <c r="F65" s="20"/>
-    </row>
-    <row r="66" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B65" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" s="20"/>
+    </row>
+    <row r="66" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
         <v>248.02</v>
       </c>
-      <c r="B66" s="20">
+      <c r="B66" t="b">
+        <v>0</v>
+      </c>
+      <c r="C66" s="20">
         <v>5724</v>
       </c>
-      <c r="C66" s="20">
+      <c r="D66" s="20">
         <v>1780</v>
       </c>
-      <c r="D66" s="20">
+      <c r="E66" s="20">
         <v>310</v>
       </c>
-      <c r="E66" s="20">
+      <c r="F66" s="20">
         <v>550</v>
       </c>
-      <c r="F66" s="20">
-        <v>0</v>
-      </c>
       <c r="G66" s="20">
+        <v>0</v>
+      </c>
+      <c r="H66" s="20">
         <v>925</v>
       </c>
-      <c r="H66" s="15">
+      <c r="I66" s="15">
         <v>5</v>
       </c>
-      <c r="I66" s="20">
+      <c r="J66" s="20">
         <v>790</v>
       </c>
-      <c r="J66" s="15">
+      <c r="K66" s="15">
         <v>75</v>
       </c>
-      <c r="K66" s="20">
+      <c r="L66" s="20">
         <v>50</v>
       </c>
-      <c r="L66" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M66" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
         <v>248.03</v>
       </c>
-      <c r="B67" s="20">
+      <c r="B67" t="b">
+        <v>0</v>
+      </c>
+      <c r="C67" s="20">
         <v>2789</v>
       </c>
-      <c r="C67" s="20">
+      <c r="D67" s="20">
         <v>785</v>
       </c>
-      <c r="D67" s="20">
+      <c r="E67" s="20">
         <v>325</v>
       </c>
-      <c r="E67" s="20">
-        <v>0</v>
-      </c>
       <c r="F67" s="20">
         <v>0</v>
       </c>
       <c r="G67" s="20">
+        <v>0</v>
+      </c>
+      <c r="H67" s="20">
         <v>465</v>
       </c>
-      <c r="H67" s="15">
+      <c r="I67" s="15">
         <v>40</v>
       </c>
-      <c r="I67" s="20">
+      <c r="J67" s="20">
         <v>275</v>
       </c>
-      <c r="J67" s="15">
+      <c r="K67" s="15">
         <v>115</v>
       </c>
-      <c r="K67" s="20">
+      <c r="L67" s="20">
         <v>40</v>
       </c>
-      <c r="L67" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M67" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
         <v>248.04</v>
       </c>
-      <c r="B68" s="20">
+      <c r="B68" t="b">
+        <v>0</v>
+      </c>
+      <c r="C68" s="20">
         <v>5359</v>
       </c>
-      <c r="C68" s="20">
+      <c r="D68" s="20">
         <v>1650</v>
       </c>
-      <c r="D68" s="20">
+      <c r="E68" s="20">
         <v>500</v>
       </c>
-      <c r="E68" s="20">
+      <c r="F68" s="20">
         <v>730</v>
       </c>
-      <c r="F68" s="20">
-        <v>0</v>
-      </c>
       <c r="G68" s="20">
+        <v>0</v>
+      </c>
+      <c r="H68" s="20">
         <v>420</v>
       </c>
-      <c r="H68" s="15">
-        <v>0</v>
-      </c>
-      <c r="I68" s="20">
+      <c r="I68" s="15">
+        <v>0</v>
+      </c>
+      <c r="J68" s="20">
         <v>145</v>
       </c>
-      <c r="J68" s="15">
+      <c r="K68" s="15">
         <v>250</v>
       </c>
-      <c r="K68" s="20">
+      <c r="L68" s="20">
         <v>30</v>
       </c>
-      <c r="L68" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M68" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
         <v>248.05</v>
       </c>
-      <c r="B69" s="20">
+      <c r="B69" t="b">
+        <v>0</v>
+      </c>
+      <c r="C69" s="20">
         <v>4475</v>
       </c>
-      <c r="C69" s="20">
+      <c r="D69" s="20">
         <v>1295</v>
       </c>
-      <c r="D69" s="20">
+      <c r="E69" s="20">
         <v>500</v>
       </c>
-      <c r="E69" s="20">
-        <v>0</v>
-      </c>
       <c r="F69" s="20">
         <v>0</v>
       </c>
       <c r="G69" s="20">
+        <v>0</v>
+      </c>
+      <c r="H69" s="20">
         <v>800</v>
       </c>
-      <c r="H69" s="15">
+      <c r="I69" s="15">
         <v>100</v>
       </c>
-      <c r="I69" s="20">
+      <c r="J69" s="20">
         <v>285</v>
       </c>
-      <c r="J69" s="15">
+      <c r="K69" s="15">
         <v>230</v>
       </c>
-      <c r="K69" s="20">
+      <c r="L69" s="20">
         <v>180</v>
       </c>
-      <c r="L69" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M69" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
         <v>249.01</v>
       </c>
-      <c r="B70" s="20">
+      <c r="B70" t="b">
+        <v>0</v>
+      </c>
+      <c r="C70" s="20">
         <v>4812</v>
       </c>
-      <c r="C70" s="20">
+      <c r="D70" s="20">
         <v>1305</v>
       </c>
-      <c r="D70" s="20">
+      <c r="E70" s="20">
         <v>810</v>
       </c>
-      <c r="E70" s="20">
+      <c r="F70" s="20">
         <v>5</v>
       </c>
-      <c r="F70" s="20">
-        <v>0</v>
-      </c>
       <c r="G70" s="20">
+        <v>0</v>
+      </c>
+      <c r="H70" s="20">
         <v>500</v>
       </c>
-      <c r="H70" s="15">
+      <c r="I70" s="15">
         <v>70</v>
       </c>
-      <c r="I70" s="20">
+      <c r="J70" s="20">
         <v>110</v>
       </c>
-      <c r="J70" s="15">
+      <c r="K70" s="15">
         <v>305</v>
       </c>
-      <c r="K70" s="20">
+      <c r="L70" s="20">
         <v>15</v>
       </c>
-      <c r="L70" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M70" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="19">
         <v>249.02</v>
       </c>
-      <c r="F71" s="20"/>
-    </row>
-    <row r="72" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" s="20"/>
+    </row>
+    <row r="72" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
         <v>249.03</v>
       </c>
-      <c r="B72" s="20">
+      <c r="B72" t="b">
+        <v>0</v>
+      </c>
+      <c r="C72" s="20">
         <v>5771</v>
       </c>
-      <c r="C72" s="20">
+      <c r="D72" s="20">
         <v>1585</v>
       </c>
-      <c r="D72" s="20">
+      <c r="E72" s="20">
         <v>685</v>
       </c>
-      <c r="E72" s="20">
+      <c r="F72" s="20">
         <v>5</v>
       </c>
-      <c r="F72" s="20">
-        <v>0</v>
-      </c>
       <c r="G72" s="20">
+        <v>0</v>
+      </c>
+      <c r="H72" s="20">
         <v>900</v>
       </c>
-      <c r="H72" s="15">
+      <c r="I72" s="15">
         <v>50</v>
       </c>
-      <c r="I72" s="20">
+      <c r="J72" s="20">
         <v>375</v>
       </c>
-      <c r="J72" s="15">
+      <c r="K72" s="15">
         <v>400</v>
       </c>
-      <c r="K72" s="20">
+      <c r="L72" s="20">
         <v>75</v>
       </c>
-      <c r="L72" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M72" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
         <v>249.04</v>
       </c>
-      <c r="B73" s="20">
+      <c r="B73" t="b">
+        <v>0</v>
+      </c>
+      <c r="C73" s="20">
         <v>3283</v>
       </c>
-      <c r="C73" s="20">
+      <c r="D73" s="20">
         <v>915</v>
       </c>
-      <c r="D73" s="20">
+      <c r="E73" s="20">
         <v>485</v>
       </c>
-      <c r="E73" s="20">
+      <c r="F73" s="20">
         <v>130</v>
       </c>
-      <c r="F73" s="20">
-        <v>0</v>
-      </c>
       <c r="G73" s="20">
+        <v>0</v>
+      </c>
+      <c r="H73" s="20">
         <v>300</v>
       </c>
-      <c r="H73" s="15">
+      <c r="I73" s="15">
         <v>70</v>
       </c>
-      <c r="I73" s="20">
+      <c r="J73" s="20">
         <v>5</v>
       </c>
-      <c r="J73" s="15">
+      <c r="K73" s="15">
         <v>220</v>
       </c>
-      <c r="K73" s="20">
+      <c r="L73" s="20">
         <v>15</v>
       </c>
-      <c r="L73" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M73" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
         <v>249.05</v>
       </c>
-      <c r="B74" s="20">
+      <c r="B74" t="b">
+        <v>0</v>
+      </c>
+      <c r="C74" s="20">
         <v>5518</v>
       </c>
-      <c r="C74" s="20">
+      <c r="D74" s="20">
         <v>1475</v>
       </c>
-      <c r="D74" s="20">
+      <c r="E74" s="20">
         <v>85</v>
       </c>
-      <c r="E74" s="20">
+      <c r="F74" s="20">
         <v>1190</v>
       </c>
-      <c r="F74" s="20">
-        <v>0</v>
-      </c>
       <c r="G74" s="20">
+        <v>0</v>
+      </c>
+      <c r="H74" s="20">
         <v>205</v>
       </c>
-      <c r="H74" s="15">
+      <c r="I74" s="15">
         <v>20</v>
       </c>
-      <c r="I74" s="20">
+      <c r="J74" s="20">
         <v>130</v>
       </c>
-      <c r="J74" s="15">
+      <c r="K74" s="15">
         <v>55</v>
       </c>
-      <c r="K74" s="20">
+      <c r="L74" s="20">
         <v>5</v>
       </c>
-      <c r="L74" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M74" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
         <v>250.01</v>
       </c>
-      <c r="B75" s="20">
+      <c r="B75" t="b">
+        <v>0</v>
+      </c>
+      <c r="C75" s="20">
         <v>5172</v>
       </c>
-      <c r="C75" s="20">
+      <c r="D75" s="20">
         <v>1490</v>
       </c>
-      <c r="D75" s="20">
+      <c r="E75" s="20">
         <v>700</v>
       </c>
-      <c r="E75" s="20">
+      <c r="F75" s="20">
         <v>235</v>
       </c>
-      <c r="F75" s="20">
-        <v>0</v>
-      </c>
       <c r="G75" s="20">
+        <v>0</v>
+      </c>
+      <c r="H75" s="20">
         <v>555</v>
       </c>
-      <c r="H75" s="15">
+      <c r="I75" s="15">
         <v>210</v>
       </c>
-      <c r="I75" s="20">
+      <c r="J75" s="20">
         <v>55</v>
       </c>
-      <c r="J75" s="15">
+      <c r="K75" s="15">
         <v>140</v>
       </c>
-      <c r="K75" s="20">
+      <c r="L75" s="20">
         <v>155</v>
       </c>
-      <c r="L75" s="15">
+      <c r="M75" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
         <v>250.02</v>
       </c>
-      <c r="B76" s="20">
+      <c r="B76" t="b">
+        <v>0</v>
+      </c>
+      <c r="C76" s="20">
         <v>4966</v>
       </c>
-      <c r="C76" s="20">
+      <c r="D76" s="20">
         <v>1730</v>
       </c>
-      <c r="D76" s="20">
+      <c r="E76" s="20">
         <v>920</v>
       </c>
-      <c r="E76" s="20">
+      <c r="F76" s="20">
         <v>430</v>
       </c>
-      <c r="F76" s="20">
-        <v>0</v>
-      </c>
       <c r="G76" s="20">
+        <v>0</v>
+      </c>
+      <c r="H76" s="20">
         <v>375</v>
       </c>
-      <c r="H76" s="15">
+      <c r="I76" s="15">
         <v>90</v>
       </c>
-      <c r="I76" s="20">
-        <v>0</v>
-      </c>
-      <c r="J76" s="15">
+      <c r="J76" s="20">
+        <v>0</v>
+      </c>
+      <c r="K76" s="15">
         <v>170</v>
       </c>
-      <c r="K76" s="20">
+      <c r="L76" s="20">
         <v>115</v>
       </c>
-      <c r="L76" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M76" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="19">
         <v>250.03</v>
       </c>
-      <c r="F77" s="20"/>
-    </row>
-    <row r="78" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" s="20"/>
+    </row>
+    <row r="78" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
         <v>250.04</v>
       </c>
-      <c r="B78" s="20">
+      <c r="B78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C78" s="20">
         <v>6031</v>
       </c>
-      <c r="C78" s="20">
+      <c r="D78" s="20">
         <v>1955</v>
       </c>
-      <c r="D78" s="20">
-        <v>0</v>
-      </c>
       <c r="E78" s="20">
+        <v>0</v>
+      </c>
+      <c r="F78" s="20">
         <v>1955</v>
       </c>
-      <c r="F78" s="20">
-        <v>0</v>
-      </c>
       <c r="G78" s="20">
         <v>0</v>
       </c>
-      <c r="H78" s="15">
-        <v>0</v>
-      </c>
-      <c r="I78" s="20">
-        <v>0</v>
-      </c>
-      <c r="J78" s="15">
-        <v>0</v>
-      </c>
-      <c r="K78" s="20">
-        <v>0</v>
-      </c>
-      <c r="L78" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="H78" s="20">
+        <v>0</v>
+      </c>
+      <c r="I78" s="15">
+        <v>0</v>
+      </c>
+      <c r="J78" s="20">
+        <v>0</v>
+      </c>
+      <c r="K78" s="15">
+        <v>0</v>
+      </c>
+      <c r="L78" s="20">
+        <v>0</v>
+      </c>
+      <c r="M78" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
         <v>250.05</v>
       </c>
-      <c r="B79" s="20">
+      <c r="B79" t="b">
+        <v>0</v>
+      </c>
+      <c r="C79" s="20">
         <v>7420</v>
       </c>
-      <c r="C79" s="20">
+      <c r="D79" s="20">
         <v>2150</v>
       </c>
-      <c r="D79" s="20">
-        <v>0</v>
-      </c>
       <c r="E79" s="20">
+        <v>0</v>
+      </c>
+      <c r="F79" s="20">
         <v>2145</v>
       </c>
-      <c r="F79" s="20">
-        <v>0</v>
-      </c>
       <c r="G79" s="20">
+        <v>0</v>
+      </c>
+      <c r="H79" s="20">
         <v>5</v>
       </c>
-      <c r="H79" s="15">
+      <c r="I79" s="15">
         <v>5</v>
       </c>
-      <c r="I79" s="20">
-        <v>0</v>
-      </c>
-      <c r="J79" s="15">
-        <v>0</v>
-      </c>
-      <c r="K79" s="20">
-        <v>0</v>
-      </c>
-      <c r="L79" s="15">
+      <c r="J79" s="20">
+        <v>0</v>
+      </c>
+      <c r="K79" s="15">
+        <v>0</v>
+      </c>
+      <c r="L79" s="20">
+        <v>0</v>
+      </c>
+      <c r="M79" s="15">
         <v>0</v>
       </c>
     </row>

</xml_diff>